<commit_message>
luiz felipe é um viadão
</commit_message>
<xml_diff>
--- a/Relatorio de Não Conformidade  - NoIdea.xlsx
+++ b/Relatorio de Não Conformidade  - NoIdea.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2650831723029\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2650831723029\Desktop\Nova pasta\SearchSoundOficial\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -392,7 +392,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -457,6 +457,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF9999FF"/>
         <bgColor rgb="FFCC99FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -541,151 +547,154 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1039,8 +1048,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1049,7 +1058,7 @@
     <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="28.5703125" customWidth="1"/>
     <col min="4" max="4" width="42.85546875" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125"/>
     <col min="7" max="7" width="95.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="98.85546875" bestFit="1" customWidth="1"/>
@@ -1064,968 +1073,968 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
     </row>
     <row r="2" spans="1:18" ht="34.700000000000003" hidden="1" customHeight="1">
-      <c r="A2" s="15">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="20">
+      <c r="J2" s="10">
         <v>43362</v>
       </c>
-      <c r="K2" s="20">
+      <c r="K2" s="10">
         <v>43388</v>
       </c>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16" t="s">
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="O2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
     </row>
     <row r="3" spans="1:18" ht="35.450000000000003" hidden="1" customHeight="1">
-      <c r="A3" s="15">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="20">
+      <c r="J3" s="10">
         <v>43362</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3" s="10">
         <v>43388</v>
       </c>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16" t="s">
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="O3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
-      <c r="R3" s="23"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
     </row>
     <row r="4" spans="1:18" ht="33.4" hidden="1" customHeight="1">
-      <c r="A4" s="15">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="20">
+      <c r="J4" s="10">
         <v>43362</v>
       </c>
-      <c r="K4" s="20">
+      <c r="K4" s="10">
         <v>43388</v>
       </c>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16" t="s">
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="21" t="s">
+      <c r="O4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
     </row>
     <row r="5" spans="1:18" ht="33.4" hidden="1" customHeight="1">
-      <c r="A5" s="15">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="I5" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="10">
         <v>43362</v>
       </c>
-      <c r="K5" s="20">
+      <c r="K5" s="10">
         <v>43388</v>
       </c>
-      <c r="L5" s="16"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="16" t="s">
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O5" s="21" t="s">
+      <c r="O5" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="22"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
     </row>
     <row r="6" spans="1:18" ht="25.5" hidden="1">
-      <c r="A6" s="15">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="I6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="10">
         <v>43362</v>
       </c>
-      <c r="K6" s="20">
+      <c r="K6" s="10">
         <v>43388</v>
       </c>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16" t="s">
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O6" s="21" t="s">
+      <c r="O6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
-      <c r="R6" s="22"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
     </row>
     <row r="7" spans="1:18" ht="28.7" hidden="1" customHeight="1">
-      <c r="A7" s="10">
+      <c r="A7" s="47">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="46">
         <v>43362</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="38">
         <v>43388</v>
       </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3" t="s">
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="O7" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
     </row>
     <row r="8" spans="1:18" hidden="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="22"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
     </row>
     <row r="9" spans="1:18" hidden="1">
-      <c r="A9" s="10">
+      <c r="A9" s="47">
         <v>7</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="46">
         <v>43362</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="38">
         <v>43388</v>
       </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3" t="s">
+      <c r="L9" s="39"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="O9" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="22"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
     </row>
     <row r="10" spans="1:18" hidden="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="6" t="s">
+      <c r="A10" s="47"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="5"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
     </row>
     <row r="11" spans="1:18" ht="12.75" customHeight="1">
-      <c r="A11" s="10">
+      <c r="A11" s="47">
         <v>8</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="46">
         <v>43362</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="38">
         <v>43388</v>
       </c>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3" t="s">
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="O11" s="48" t="s">
+      <c r="O11" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="22"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
     </row>
     <row r="12" spans="1:18" ht="23.85" hidden="1" customHeight="1">
-      <c r="A12" s="10"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="6" t="s">
+      <c r="A12" s="47"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="46">
         <v>43363</v>
       </c>
-      <c r="K12" s="4"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="49"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="22"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39"/>
+      <c r="N12" s="39"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
     </row>
     <row r="13" spans="1:18" ht="25.5">
-      <c r="A13" s="15">
+      <c r="A13" s="5">
         <v>11</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="I13" s="19" t="s">
+      <c r="I13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J13" s="27">
+      <c r="J13" s="17">
         <v>43364</v>
       </c>
-      <c r="K13" s="20">
+      <c r="K13" s="10">
         <v>43398</v>
       </c>
-      <c r="L13" s="16"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="18" t="s">
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="O13" s="21" t="s">
+      <c r="O13" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="22"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
     </row>
     <row r="14" spans="1:18" ht="13.5">
-      <c r="A14" s="15">
+      <c r="A14" s="5">
         <v>12</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F14" s="24" t="s">
+      <c r="F14" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I14" s="26" t="s">
+      <c r="I14" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="27">
+      <c r="J14" s="17">
         <v>43365</v>
       </c>
-      <c r="K14" s="20">
+      <c r="K14" s="10">
         <v>43398</v>
       </c>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="18" t="s">
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="O14" s="21" t="s">
+      <c r="O14" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="22"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
     </row>
     <row r="15" spans="1:18" ht="13.5" hidden="1">
-      <c r="A15" s="15">
+      <c r="A15" s="5">
         <v>13</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="F15" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="27">
+      <c r="J15" s="17">
         <v>43366</v>
       </c>
-      <c r="K15" s="20">
+      <c r="K15" s="10">
         <v>43398</v>
       </c>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
-      <c r="N15" s="18" t="s">
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="O15" s="21" t="s">
+      <c r="O15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="22"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
     </row>
     <row r="16" spans="1:18" ht="13.5">
-      <c r="A16" s="15">
+      <c r="A16" s="5">
         <v>14</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F16" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H16" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="I16" s="28" t="s">
+      <c r="I16" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="J16" s="29" t="s">
+      <c r="J16" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="K16" s="20">
+      <c r="K16" s="10">
         <v>43403</v>
       </c>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="18" t="s">
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="O16" s="16" t="s">
+      <c r="O16" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
     </row>
     <row r="17" spans="1:18" ht="25.5" hidden="1">
-      <c r="A17" s="15">
+      <c r="A17" s="5">
         <v>15</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="F17" s="24" t="s">
+      <c r="F17" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="18" t="s">
+      <c r="G17" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J17" s="29" t="s">
+      <c r="J17" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="K17" s="20">
+      <c r="K17" s="10">
         <v>43403</v>
       </c>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="18" t="s">
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="O17" s="30" t="s">
+      <c r="O17" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
     </row>
     <row r="18" spans="1:18" ht="38.25">
-      <c r="A18" s="15">
+      <c r="A18" s="5">
         <v>16</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="24" t="s">
+      <c r="F18" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="18" t="s">
+      <c r="G18" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="H18" s="18" t="s">
+      <c r="H18" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="I18" s="28" t="s">
+      <c r="I18" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="J18" s="29" t="s">
+      <c r="J18" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="K18" s="20">
+      <c r="K18" s="10">
         <v>43403</v>
       </c>
-      <c r="L18" s="16"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="18" t="s">
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="O18" s="30" t="s">
+      <c r="O18" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
     </row>
     <row r="19" spans="1:18" ht="13.5" hidden="1">
-      <c r="A19" s="15">
+      <c r="A19" s="5">
         <v>17</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="F19" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="18" t="s">
+      <c r="G19" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="H19" s="18" t="s">
+      <c r="H19" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="I19" s="19" t="s">
+      <c r="I19" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J19" s="29" t="s">
+      <c r="J19" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="K19" s="20">
+      <c r="K19" s="10">
         <v>43403</v>
       </c>
-      <c r="L19" s="16"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="18" t="s">
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="O19" s="30" t="s">
+      <c r="O19" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
     </row>
     <row r="20" spans="1:18" ht="13.5">
-      <c r="A20" s="15">
+      <c r="A20" s="5">
         <v>18</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="F20" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="I20" s="28" t="s">
+      <c r="I20" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="J20" s="29" t="s">
+      <c r="J20" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="K20" s="20">
+      <c r="K20" s="10">
         <v>43403</v>
       </c>
-      <c r="L20" s="16"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="18" t="s">
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="O20" s="16" t="s">
+      <c r="O20" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="22"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
     </row>
     <row r="21" spans="1:18" ht="13.5" hidden="1">
-      <c r="A21" s="15">
+      <c r="A21" s="5">
         <v>19</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="24" t="s">
+      <c r="F21" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="18" t="s">
+      <c r="G21" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="H21" s="18" t="s">
+      <c r="H21" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="I21" s="19" t="s">
+      <c r="I21" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J21" s="29" t="s">
+      <c r="J21" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="K21" s="20">
+      <c r="K21" s="10">
         <v>43403</v>
       </c>
-      <c r="L21" s="16"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="18" t="s">
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="O21" s="30" t="s">
+      <c r="O21" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="P21" s="22"/>
-      <c r="Q21" s="22"/>
-      <c r="R21" s="22"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
     </row>
     <row r="22" spans="1:18" ht="13.5" hidden="1">
-      <c r="A22" s="15">
+      <c r="A22" s="5">
         <v>20</v>
       </c>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="35"/>
-      <c r="O22" s="36"/>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="22"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="25"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
     </row>
     <row r="23" spans="1:18" ht="13.5" hidden="1">
-      <c r="A23" s="15">
+      <c r="A23" s="5">
         <v>21</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="35"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="37"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="22"/>
-      <c r="R23" s="22"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
     </row>
     <row r="24" spans="1:18" ht="13.5" hidden="1">
-      <c r="A24" s="15">
+      <c r="A24" s="5">
         <v>22</v>
       </c>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="37"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="22"/>
-      <c r="R24" s="22"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
     </row>
     <row r="1048576" ht="12.75" customHeight="1"/>
   </sheetData>
@@ -2037,51 +2046,51 @@
     </filterColumn>
   </autoFilter>
   <mergeCells count="45">
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="M9:M10"/>
+    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="O9:O10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="L11:L12"/>
     <mergeCell ref="M11:M12"/>
     <mergeCell ref="N11:N12"/>
     <mergeCell ref="O11:O12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="M9:M10"/>
-    <mergeCell ref="N9:N10"/>
-    <mergeCell ref="O9:O10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2105,45 +2114,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4">
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="39"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:4">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="41"/>
+      <c r="C2" s="31"/>
       <c r="D2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="3" spans="2:4">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="41"/>
+      <c r="C3" s="31"/>
       <c r="D3" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="4" spans="2:4">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="41"/>
+      <c r="C4" s="31"/>
       <c r="D4" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="6" spans="2:4">
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="29" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:4">
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="34" t="s">
         <v>40</v>
       </c>
       <c r="D7" t="s">
@@ -2151,7 +2160,7 @@
       </c>
     </row>
     <row r="8" spans="2:4">
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="35" t="s">
         <v>22</v>
       </c>
       <c r="D8" t="s">
@@ -2159,7 +2168,7 @@
       </c>
     </row>
     <row r="9" spans="2:4">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="36" t="s">
         <v>96</v>
       </c>
       <c r="D9" t="s">
@@ -2167,7 +2176,7 @@
       </c>
     </row>
     <row r="10" spans="2:4">
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="37" t="s">
         <v>98</v>
       </c>
       <c r="D10" t="s">

</xml_diff>